<commit_message>
found an error in computing the average for texting on Android.
</commit_message>
<xml_diff>
--- a/usability-metrics/CMSI-370-assignment-0918-data.xlsx
+++ b/usability-metrics/CMSI-370-assignment-0918-data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="-40" windowWidth="27960" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="-20" yWindow="-20" windowWidth="21600" windowHeight="14620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,147 +19,146 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="33">
-  <si>
-    <t>Iphone</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>HTC Evo 4g</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="33">
   <si>
     <t>Learnability</t>
   </si>
   <si>
     <t>Learnability</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Satisfaction</t>
   </si>
   <si>
     <t>Satisfaction</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Efficiency1</t>
   </si>
   <si>
     <t>Efficiency1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Efficiency2</t>
   </si>
   <si>
     <t>Efficiency2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Efficiency3</t>
   </si>
   <si>
     <t>Efficiency3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>TZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ringtone</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TZ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TZ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>ED</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TB</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>C</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>M</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>TZ</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>KF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>KF</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AD</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ma</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>VL</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>AVERAGE</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Call</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>Text</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ringtone</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Call</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ED</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TB</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>C</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>M</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>M</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>TZ</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>KF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>KF</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ma</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>VL</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Android</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>iPhone</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
+      <sz val="10"/>
+      <name val="Verdana"/>
+    </font>
+    <font>
+      <b/>
       <sz val="10"/>
       <name val="Verdana"/>
     </font>
@@ -190,7 +189,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -523,75 +522,75 @@
   <dimension ref="A1:R31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="A1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" t="s">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>4</v>
+      </c>
+      <c r="J2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" t="s">
+        <v>11</v>
+      </c>
+      <c r="N2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I1" t="s">
-        <v>6</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" t="s">
-        <v>15</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="Q2" t="s">
+        <v>9</v>
+      </c>
+      <c r="R2" t="s">
         <v>3</v>
-      </c>
-      <c r="O1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P1" t="s">
-        <v>9</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>11</v>
-      </c>
-      <c r="R1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
-      <c r="A3" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>8.1999999999999993</v>
@@ -606,7 +605,7 @@
         <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I4">
         <v>21.5</v>
@@ -621,7 +620,7 @@
         <v>8</v>
       </c>
       <c r="M4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="O4">
         <v>9</v>
@@ -638,7 +637,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>8.1999999999999993</v>
@@ -653,7 +652,7 @@
         <v>10</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="I5">
         <v>23.6</v>
@@ -668,7 +667,7 @@
         <v>8</v>
       </c>
       <c r="M5" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="O5">
         <v>6</v>
@@ -685,7 +684,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B6">
         <v>14.4</v>
@@ -694,7 +693,7 @@
         <v>7</v>
       </c>
       <c r="G6" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="H6">
         <v>38.4</v>
@@ -703,7 +702,7 @@
         <v>5</v>
       </c>
       <c r="M6" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="N6">
         <v>26.7</v>
@@ -714,7 +713,7 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B7">
         <v>11.4</v>
@@ -723,7 +722,7 @@
         <v>9</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H7">
         <v>51.4</v>
@@ -732,7 +731,7 @@
         <v>4</v>
       </c>
       <c r="M7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="N7">
         <v>38.5</v>
@@ -743,7 +742,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="C8">
         <v>9.9</v>
@@ -758,7 +757,7 @@
         <v>9</v>
       </c>
       <c r="G8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="I8">
         <v>18.5</v>
@@ -773,7 +772,7 @@
         <v>9</v>
       </c>
       <c r="M8" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="O8">
         <v>8.8000000000000007</v>
@@ -790,7 +789,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="C9">
         <v>9.6999999999999993</v>
@@ -805,7 +804,7 @@
         <v>10</v>
       </c>
       <c r="G9" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="I9">
         <v>22.2</v>
@@ -820,7 +819,7 @@
         <v>10</v>
       </c>
       <c r="M9" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="O9">
         <v>11.4</v>
@@ -837,7 +836,7 @@
     </row>
     <row r="10" spans="1:18">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C10">
         <v>13.2</v>
@@ -852,7 +851,7 @@
         <v>9</v>
       </c>
       <c r="G10" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="I10">
         <v>21.1</v>
@@ -867,7 +866,7 @@
         <v>9</v>
       </c>
       <c r="M10" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="O10">
         <v>30.4</v>
@@ -884,7 +883,7 @@
     </row>
     <row r="11" spans="1:18">
       <c r="A11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -893,7 +892,7 @@
         <v>8</v>
       </c>
       <c r="G11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="H11">
         <v>21.8</v>
@@ -902,7 +901,7 @@
         <v>7</v>
       </c>
       <c r="M11" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="N11">
         <v>12.3</v>
@@ -912,6 +911,9 @@
       </c>
     </row>
     <row r="12" spans="1:18">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
       <c r="B12">
         <f>AVERAGE(B4:B11)</f>
         <v>11.933333333333332</v>
@@ -932,6 +934,9 @@
         <f t="shared" si="0"/>
         <v>8.875</v>
       </c>
+      <c r="G12" t="s">
+        <v>28</v>
+      </c>
       <c r="H12">
         <f>AVERAGE(H4:H11)</f>
         <v>37.199999999999996</v>
@@ -951,6 +956,9 @@
       <c r="L12">
         <f t="shared" ref="L12" si="4">AVERAGE(L4:L11)</f>
         <v>7.5</v>
+      </c>
+      <c r="M12" t="s">
+        <v>28</v>
       </c>
       <c r="N12">
         <f>AVERAGE(N4:N11)</f>
@@ -987,70 +995,70 @@
         <v>8.2933333333333312</v>
       </c>
     </row>
+    <row r="18" spans="1:18">
+      <c r="A18" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
     <row r="19" spans="1:18">
-      <c r="A19" t="s">
-        <v>16</v>
+      <c r="A19" s="1" t="s">
+        <v>29</v>
       </c>
       <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" t="s">
         <v>2</v>
       </c>
-      <c r="C19" t="s">
+      <c r="G19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="H19" t="s">
+        <v>0</v>
+      </c>
+      <c r="I19" t="s">
+        <v>4</v>
+      </c>
+      <c r="J19" t="s">
         <v>6</v>
       </c>
-      <c r="D19" t="s">
+      <c r="K19" t="s">
         <v>8</v>
       </c>
-      <c r="E19" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" t="s">
+      <c r="L19" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="M19" t="s">
+        <v>11</v>
+      </c>
+      <c r="N19" t="s">
+        <v>0</v>
+      </c>
+      <c r="O19" t="s">
         <v>4</v>
       </c>
-      <c r="G19" t="s">
-        <v>14</v>
-      </c>
-      <c r="H19" t="s">
+      <c r="P19" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>8</v>
+      </c>
+      <c r="R19" t="s">
         <v>2</v>
-      </c>
-      <c r="I19" t="s">
-        <v>6</v>
-      </c>
-      <c r="J19" t="s">
-        <v>8</v>
-      </c>
-      <c r="K19" t="s">
-        <v>10</v>
-      </c>
-      <c r="L19" t="s">
-        <v>4</v>
-      </c>
-      <c r="M19" t="s">
-        <v>15</v>
-      </c>
-      <c r="N19" t="s">
-        <v>2</v>
-      </c>
-      <c r="O19" t="s">
-        <v>6</v>
-      </c>
-      <c r="P19" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q19" t="s">
-        <v>10</v>
-      </c>
-      <c r="R19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:18">
-      <c r="A20" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:18">
       <c r="A21" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B21">
         <v>17.7</v>
@@ -1059,7 +1067,7 @@
         <v>8</v>
       </c>
       <c r="G21" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="H21">
         <v>55.1</v>
@@ -1068,7 +1076,7 @@
         <v>6</v>
       </c>
       <c r="M21" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="N21">
         <v>7.8</v>
@@ -1079,7 +1087,7 @@
     </row>
     <row r="22" spans="1:18">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B22">
         <v>11.2</v>
@@ -1088,7 +1096,7 @@
         <v>9</v>
       </c>
       <c r="G22" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="H22">
         <v>31.6</v>
@@ -1097,7 +1105,7 @@
         <v>7</v>
       </c>
       <c r="M22" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="N22">
         <v>25.6</v>
@@ -1108,7 +1116,7 @@
     </row>
     <row r="23" spans="1:18">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B23">
         <v>16.2</v>
@@ -1117,16 +1125,16 @@
         <v>7</v>
       </c>
       <c r="G23" t="s">
-        <v>20</v>
-      </c>
-      <c r="H23" s="1">
-        <v>8.7384259259259262E-4</v>
+        <v>15</v>
+      </c>
+      <c r="H23">
+        <v>75</v>
       </c>
       <c r="L23">
         <v>7</v>
       </c>
       <c r="M23" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="N23">
         <v>23</v>
@@ -1137,7 +1145,7 @@
     </row>
     <row r="24" spans="1:18">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="C24">
         <v>11</v>
@@ -1152,7 +1160,7 @@
         <v>10</v>
       </c>
       <c r="G24" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="I24">
         <v>38.299999999999997</v>
@@ -1167,7 +1175,7 @@
         <v>7</v>
       </c>
       <c r="M24" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="O24">
         <v>18.7</v>
@@ -1184,7 +1192,7 @@
     </row>
     <row r="25" spans="1:18">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B25">
         <v>16.8</v>
@@ -1193,7 +1201,7 @@
         <v>6</v>
       </c>
       <c r="G25" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="H25">
         <v>58.3</v>
@@ -1202,7 +1210,7 @@
         <v>3</v>
       </c>
       <c r="M25" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="N25">
         <v>18.5</v>
@@ -1213,7 +1221,7 @@
     </row>
     <row r="26" spans="1:18">
       <c r="A26" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B26">
         <v>14.6</v>
@@ -1222,7 +1230,7 @@
         <v>8.5</v>
       </c>
       <c r="G26" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="H26">
         <v>39</v>
@@ -1231,7 +1239,7 @@
         <v>7</v>
       </c>
       <c r="M26" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="N26">
         <v>41.5</v>
@@ -1242,7 +1250,7 @@
     </row>
     <row r="27" spans="1:18">
       <c r="A27" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B27">
         <v>15.3</v>
@@ -1251,7 +1259,7 @@
         <v>8</v>
       </c>
       <c r="G27" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H27">
         <v>38.700000000000003</v>
@@ -1260,7 +1268,7 @@
         <v>6</v>
       </c>
       <c r="M27" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="N27">
         <v>32</v>
@@ -1271,7 +1279,7 @@
     </row>
     <row r="28" spans="1:18">
       <c r="A28" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B28">
         <v>18.399999999999999</v>
@@ -1280,7 +1288,7 @@
         <v>5</v>
       </c>
       <c r="G28" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="H28">
         <v>53.9</v>
@@ -1289,7 +1297,7 @@
         <v>2</v>
       </c>
       <c r="M28" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="N28">
         <v>11</v>
@@ -1300,7 +1308,7 @@
     </row>
     <row r="29" spans="1:18">
       <c r="A29" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="C29">
         <v>12.5</v>
@@ -1315,7 +1323,7 @@
         <v>8</v>
       </c>
       <c r="G29" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="I29">
         <v>19.7</v>
@@ -1330,7 +1338,7 @@
         <v>8</v>
       </c>
       <c r="M29" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="O29">
         <v>9.6999999999999993</v>
@@ -1346,6 +1354,9 @@
       </c>
     </row>
     <row r="30" spans="1:18">
+      <c r="A30" t="s">
+        <v>28</v>
+      </c>
       <c r="B30">
         <f>AVERAGE(B22:B29)</f>
         <v>15.416666666666666</v>
@@ -1366,9 +1377,12 @@
         <f t="shared" ref="F30" si="12">AVERAGE(F22:F29)</f>
         <v>7.6875</v>
       </c>
+      <c r="G30" t="s">
+        <v>28</v>
+      </c>
       <c r="H30">
         <f>AVERAGE(H22:H29)</f>
-        <v>36.916812307098766</v>
+        <v>49.416666666666657</v>
       </c>
       <c r="I30">
         <f t="shared" ref="I30" si="13">AVERAGE(I22:I29)</f>
@@ -1385,6 +1399,9 @@
       <c r="L30">
         <f t="shared" ref="L30" si="16">AVERAGE(L22:L29)</f>
         <v>5.875</v>
+      </c>
+      <c r="M30" t="s">
+        <v>28</v>
       </c>
       <c r="N30">
         <f>AVERAGE(N22:N29)</f>
@@ -1422,9 +1439,8 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>